<commit_message>
latest data on 1st dec
</commit_message>
<xml_diff>
--- a/data/casemapdata.xlsx
+++ b/data/casemapdata.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>156323</v>
+        <v>156896</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>186793</v>
+        <v>195988</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>206754</v>
+        <v>208952</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15572</v>
+        <v>16086</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>64533</v>
+        <v>65024</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4069</v>
+        <v>4135</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5292549</v>
+        <v>5315348</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>312674</v>
+        <v>334075</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>175813</v>
+        <v>199649</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>847408</v>
+        <v>1056613</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>537004</v>
+        <v>573974</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>22429</v>
+        <v>22655</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>276956</v>
+        <v>277389</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1570238</v>
+        <v>1574088</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>18852</v>
+        <v>23795</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>606033</v>
+        <v>640206</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1393358</v>
+        <v>1581500</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>27523</v>
+        <v>29501</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>24804</v>
+        <v>24846</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2622</v>
+        <v>2632</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>514679</v>
+        <v>529075</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>256307</v>
+        <v>268572</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>187281</v>
+        <v>194445</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>21835785</v>
+        <v>22017276</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>13446</v>
+        <v>14591</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>619284</v>
+        <v>673288</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>15103</v>
+        <v>15514</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>502979</v>
+        <v>517922</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>20106</v>
+        <v>20332</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>38228</v>
+        <v>38327</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>118787</v>
+        <v>119867</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>104348</v>
+        <v>106190</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1730818</v>
+        <v>1773959</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>11579</v>
+        <v>11666</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1699427</v>
+        <v>1743137</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>109956</v>
+        <v>110983</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5007099</v>
+        <v>5048061</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4281</v>
+        <v>4450</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>17670</v>
+        <v>18717</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>57582</v>
+        <v>57880</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>561432</v>
+        <v>565548</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>61330</v>
+        <v>61591</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>476832</v>
+        <v>570380</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>953750</v>
+        <v>960802</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>124973</v>
+        <v>129888</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1783227</v>
+        <v>1995291</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>396407</v>
+        <v>454389</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>13487</v>
+        <v>13501</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4823</v>
+        <v>5642</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>384208</v>
+        <v>402731</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>515859</v>
+        <v>523847</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>333840</v>
+        <v>350397</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>113422</v>
+        <v>118041</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>13377</v>
+        <v>13538</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>6881</v>
+        <v>7175</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>199251</v>
+        <v>217381</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>46447</v>
+        <v>46487</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>366097</v>
+        <v>370200</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>52209</v>
+        <v>52453</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>160948</v>
+        <v>174823</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>7282823</v>
+        <v>7517669</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>36020</v>
+        <v>37045</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>9973</v>
+        <v>9988</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>732965</v>
+        <v>812246</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>4684462</v>
+        <v>5400687</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>130287</v>
+        <v>130827</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>760592</v>
+        <v>878920</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>5850</v>
+        <v>5873</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>602575</v>
+        <v>613892</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>30681</v>
+        <v>30715</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>6137</v>
+        <v>6434</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>35800</v>
+        <v>37325</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>24004</v>
+        <v>24768</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>375983</v>
+        <v>377420</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>879092</v>
+        <v>998488</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>13923</v>
+        <v>16435</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>34321025</v>
+        <v>34518901</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -1627,7 +1627,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>4246174</v>
+        <v>4253412</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5954962</v>
+        <v>6077438</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>2058914</v>
+        <v>2074419</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>455346</v>
+        <v>528964</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1332247</v>
+        <v>1340435</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>4782802</v>
+        <v>4925688</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>89216</v>
+        <v>90705</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>1724128</v>
+        <v>1725850</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>868493</v>
+        <v>914849</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>1024449</v>
+        <v>1046722</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>253512</v>
+        <v>254710</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>373120</v>
+        <v>418252</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>160809</v>
+        <v>161006</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>412752</v>
+        <v>413137</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>181499</v>
+        <v>182833</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>42891</v>
+        <v>62160</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>224513</v>
+        <v>246116</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>643749</v>
+        <v>659404</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>21643</v>
+        <v>21729</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>5815</v>
+        <v>5818</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>359019</v>
+        <v>367811</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>3699</v>
+        <v>4144</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>414817</v>
+        <v>455558</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>82190</v>
+        <v>85960</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>43632</v>
+        <v>43672</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>61803</v>
+        <v>61863</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>2486630</v>
+        <v>2586601</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>88277</v>
+        <v>90725</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>16195</v>
+        <v>16946</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2077,7 +2077,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>37736</v>
+        <v>38709</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>37489</v>
+        <v>38647</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>18205</v>
+        <v>18979</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>3811793</v>
+        <v>3862137</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>341675</v>
+        <v>358202</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>3424</v>
+        <v>3554</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>362772</v>
+        <v>377674</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>145936</v>
+        <v>154758</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>946766</v>
+        <v>948923</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -2227,7 +2227,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>151325</v>
+        <v>151488</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>128963</v>
+        <v>129091</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>813828</v>
+        <v>819019</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>2196598</v>
+        <v>2483084</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -2287,7 +2287,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>6973</v>
+        <v>10177</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>16699</v>
+        <v>17023</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>6399</v>
+        <v>6836</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>212359</v>
+        <v>213589</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>211755</v>
+        <v>242911</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>304318</v>
+        <v>304492</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -2377,7 +2377,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>1275158</v>
+        <v>1282195</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>473005</v>
+        <v>475997</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>31010</v>
+        <v>34442</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>461184</v>
+        <v>462198</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>2203310</v>
+        <v>2224344</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -2467,7 +2467,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>2793898</v>
+        <v>2826410</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>3045102</v>
+        <v>3345388</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>1092666</v>
+        <v>1122283</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>239646</v>
+        <v>242087</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>1676293</v>
+        <v>1762701</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>8494589</v>
+        <v>9170898</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -2557,7 +2557,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>99820</v>
+        <v>100217</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>2696</v>
+        <v>2766</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>12610</v>
+        <v>12904</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>5050</v>
+        <v>5391</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>5569</v>
+        <v>5758</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
@@ -2647,7 +2647,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>3715</v>
+        <v>3731</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>548760</v>
+        <v>549479</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
@@ -2677,7 +2677,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>73926</v>
+        <v>73968</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
@@ -2692,7 +2692,7 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>1162482</v>
+        <v>1233057</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>22301</v>
+        <v>22895</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>6398</v>
+        <v>6400</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>207975</v>
+        <v>252188</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -2752,7 +2752,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>493277</v>
+        <v>1074264</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>341699</v>
+        <v>400685</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>21998</v>
+        <v>22969</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>2922735</v>
+        <v>2929862</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -2827,7 +2827,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>12436</v>
+        <v>12638</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>5019255</v>
+        <v>5080663</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>542793</v>
+        <v>556626</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>40433</v>
+        <v>41558</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>49257</v>
+        <v>50438</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>1175425</v>
+        <v>1188735</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>881660</v>
+        <v>941218</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>44191</v>
+        <v>47212</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>16428</v>
+        <v>16529</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>17486</v>
+        <v>17489</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>26154</v>
+        <v>26227</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>1935442</v>
+        <v>2064581</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>19790</v>
+        <v>19819</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>26096</v>
+        <v>26207</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>58106</v>
+        <v>65889</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>712982</v>
+        <v>716262</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>8121196</v>
+        <v>8573524</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>46252513</v>
+        <v>47730591</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>126321</v>
+        <v>127177</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>3118140</v>
+        <v>3493203</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>740136</v>
+        <v>741433</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>9215683</v>
+        <v>9897206</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>394443</v>
+        <v>397841</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -3187,7 +3187,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>186793</v>
+        <v>191334</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -3217,7 +3217,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>409695</v>
+        <v>425213</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>939463</v>
+        <v>1094514</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
@@ -3247,7 +3247,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>454509</v>
+        <v>457950</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>9810</v>
+        <v>9955</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -3277,7 +3277,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>209781</v>
+        <v>210070</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>133091</v>
+        <v>133647</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>

</xml_diff>